<commit_message>
index, dictionary modal window
</commit_message>
<xml_diff>
--- a/src/data/vidaNR_dictonary.xlsx
+++ b/src/data/vidaNR_dictonary.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JuantxoCruz/Dropbox (Personal)/2022/2022-freelance/nacionalRe/20220119 VidaNr/webpack-vidaNr/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B496491A-7B21-9647-BA53-7B76D8D8D265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF7A398-BCA8-7841-B7FB-E1C65B2E71FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28240" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{264BACEB-9783-544A-B5AF-004F4D7AD9C4}"/>
+    <workbookView xWindow="-26320" yWindow="500" windowWidth="19100" windowHeight="17100" xr2:uid="{264BACEB-9783-544A-B5AF-004F4D7AD9C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="276">
   <si>
     <t>key</t>
   </si>
@@ -421,28 +424,6 @@
     <t>Calculate</t>
   </si>
   <si>
-    <r>
-      <t>Body </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Mass Index</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
     <t>male_upper</t>
   </si>
   <si>
@@ -467,9 +448,6 @@
     <t>First Take</t>
   </si>
   <si>
-    <t>modalSetup_header</t>
-  </si>
-  <si>
     <t>Atención</t>
   </si>
   <si>
@@ -494,9 +472,6 @@
     <t>There are erroneous or unfilled fields.</t>
   </si>
   <si>
-    <t>modalSetup_footer</t>
-  </si>
-  <si>
     <t>imcRefuseSetup_header</t>
   </si>
   <si>
@@ -692,9 +667,6 @@
     <t>Please make sure that the figure is correct in order to make the pricing.</t>
   </si>
   <si>
-    <t>modal_header_span</t>
-  </si>
-  <si>
     <t>modal_body1_span</t>
   </si>
   <si>
@@ -704,9 +676,6 @@
     <t>Patología</t>
   </si>
   <si>
-    <t>modal_footer_span</t>
-  </si>
-  <si>
     <t>Pathology</t>
   </si>
   <si>
@@ -797,12 +766,6 @@
     <t>Please choose a date again</t>
   </si>
   <si>
-    <t>warning_attention</t>
-  </si>
-  <si>
-    <t>warning_modal_footer</t>
-  </si>
-  <si>
     <t>kilos</t>
   </si>
   <si>
@@ -812,14 +775,104 @@
     <t>centímetros</t>
   </si>
   <si>
-    <t>modal_footer_copyright</t>
+    <t>modal_footer_info</t>
+  </si>
+  <si>
+    <t>modal_footer_result</t>
+  </si>
+  <si>
+    <t>modal_header_info</t>
+  </si>
+  <si>
+    <t>modal_header_result</t>
+  </si>
+  <si>
+    <t>Calculadora de recargos de seguros</t>
+  </si>
+  <si>
+    <t>Insurance surcharge calculator</t>
+  </si>
+  <si>
+    <t>Body Mass Index </t>
+  </si>
+  <si>
+    <t>h_consult_date</t>
+  </si>
+  <si>
+    <t>Consulta realizada el</t>
+  </si>
+  <si>
+    <t>h_life</t>
+  </si>
+  <si>
+    <t>Vida</t>
+  </si>
+  <si>
+    <t>h_disability</t>
+  </si>
+  <si>
+    <t>Invalidez</t>
+  </si>
+  <si>
+    <t>Accidentes</t>
+  </si>
+  <si>
+    <t>h_accidents</t>
+  </si>
+  <si>
+    <t>Enfermedad grave</t>
+  </si>
+  <si>
+    <t>h_illness</t>
+  </si>
+  <si>
+    <t>h_ilt</t>
+  </si>
+  <si>
+    <t>I.L.T.</t>
+  </si>
+  <si>
+    <t>T.W.I.</t>
+  </si>
+  <si>
+    <t>h_life_expectancy</t>
+  </si>
+  <si>
+    <t>Esperanza de vida según el agravamiento</t>
+  </si>
+  <si>
+    <t>h_print</t>
+  </si>
+  <si>
+    <t>Imprimir</t>
+  </si>
+  <si>
+    <t>Consultation made on</t>
+  </si>
+  <si>
+    <t>Life</t>
+  </si>
+  <si>
+    <t>Disability</t>
+  </si>
+  <si>
+    <t>accidents</t>
+  </si>
+  <si>
+    <t>Serious illness</t>
+  </si>
+  <si>
+    <t>Life expectancy according to aggravation</t>
+  </si>
+  <si>
+    <t>Print</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -833,12 +886,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Menlo"/>
@@ -847,12 +894,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFA31515"/>
       <name val="Menlo"/>
       <family val="2"/>
     </font>
@@ -877,13 +918,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1198,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6179227-BC3E-1D40-997E-5AA5DC3817CB}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="C101" sqref="A1:C101"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="C106" sqref="A1:C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1224,134 +1263,134 @@
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>129</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>130</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>62</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>239</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>240</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>132</v>
+      <c r="A8" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>237</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>133</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>233</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>234</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>128</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>41</v>
+        <v>73</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>68</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1378,145 +1417,145 @@
     </row>
     <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>198</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>57</v>
+        <v>201</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>58</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>200</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>61</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>62</v>
+        <v>196</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>63</v>
+        <v>199</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>64</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>69</v>
+        <v>185</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>70</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>73</v>
+        <v>227</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>71</v>
+        <v>228</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>72</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>85</v>
+        <v>230</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>74</v>
+        <v>231</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>76</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>86</v>
+        <v>218</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>75</v>
+        <v>219</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>77</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>78</v>
+        <v>221</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>79</v>
+        <v>222</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>80</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>87</v>
+        <v>224</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>81</v>
+        <v>225</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>83</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>88</v>
+        <v>215</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>82</v>
+        <v>216</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>84</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1532,797 +1571,857 @@
     </row>
     <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>99</v>
+        <v>192</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>100</v>
+        <v>193</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>98</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>101</v>
+        <v>194</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>102</v>
+        <v>195</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>103</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>111</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>104</v>
+        <v>141</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>107</v>
+        <v>3</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>115</v>
+        <v>5</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>121</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>122</v>
+        <v>183</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>123</v>
+        <v>186</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>124</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>125</v>
+        <v>184</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>126</v>
+        <v>244</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>127</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>30</v>
+        <v>152</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>31</v>
+        <v>155</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>32</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>13</v>
+        <v>151</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>15</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>16</v>
+        <v>150</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>15</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>14</v>
+        <v>147</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>15</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>14</v>
+        <v>146</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>15</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>19</v>
+        <v>144</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>14</v>
+        <v>145</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>15</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>20</v>
+        <v>162</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>14</v>
+        <v>165</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>21</v>
+        <v>161</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>14</v>
+        <v>164</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>22</v>
+        <v>160</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>14</v>
+        <v>163</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>15</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>14</v>
+        <v>113</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>14</v>
+        <v>114</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>15</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>134</v>
+      <c r="A56" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>135</v>
+        <v>6</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>136</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>137</v>
+        <v>30</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>138</v>
+        <v>31</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>139</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>140</v>
+        <v>13</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>141</v>
+        <v>14</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>142</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:3" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>143</v>
+        <v>24</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>145</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:3" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>146</v>
+        <v>25</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>218</v>
+        <v>14</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>219</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C62" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C63" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C64" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C65" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C66" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C67" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C68" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C69" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="C70" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C71" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B72" s="5" t="s">
+      <c r="C89" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C72" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C73" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="C74" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C75" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C76" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="C77" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C78" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="C79" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="C80" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C81" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C82" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C83" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C84" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="C85" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="C87" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="C88" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>220</v>
+        <v>157</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>221</v>
+        <v>159</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>222</v>
+        <v>172</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>223</v>
+        <v>156</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>224</v>
+        <v>145</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>225</v>
+        <v>166</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>226</v>
+        <v>46</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>227</v>
+        <v>47</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>228</v>
+        <v>48</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>229</v>
+        <v>44</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>230</v>
+        <v>41</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>231</v>
+        <v>42</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>232</v>
+        <v>36</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>233</v>
+        <v>37</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>234</v>
+        <v>38</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>235</v>
+        <v>177</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>236</v>
+        <v>178</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>237</v>
+        <v>181</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>238</v>
+        <v>179</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>241</v>
+        <v>176</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>242</v>
+        <v>180</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>243</v>
+        <v>182</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>244</v>
+        <v>59</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>245</v>
+        <v>60</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>139</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C99" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A100" s="1" t="s">
-        <v>248</v>
+      <c r="A100" s="2" t="s">
+        <v>254</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>219</v>
+        <v>255</v>
+      </c>
+      <c r="C100" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C101" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C102" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C103" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C105" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C106" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{E6179227-BC3E-1D40-997E-5AA5DC3817CB}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C100">
+      <sortCondition ref="A1:A100"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More wording added to excel dictionary
</commit_message>
<xml_diff>
--- a/src/data/vidaNR_dictonary.xlsx
+++ b/src/data/vidaNR_dictonary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JuantxoCruz/Dropbox (Personal)/2022/2022-freelance/nacionalRe/20220119 VidaNr/webpack-vidaNr/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743F9CC2-F2A5-5247-A903-11B68BB5406F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B0D0F8-3675-2C41-9040-C5AE58DCC99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26160" yWindow="2040" windowWidth="25860" windowHeight="17080" xr2:uid="{264BACEB-9783-544A-B5AF-004F4D7AD9C4}"/>
   </bookViews>
@@ -1409,7 +1409,7 @@
   <dimension ref="A1:C133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="D62" sqref="A1:XFD1048576"/>
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Dictionary corrections from Nacional Re and some css fixed
</commit_message>
<xml_diff>
--- a/src/data/vidaNR_dictonary.xlsx
+++ b/src/data/vidaNR_dictonary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JuantxoCruz/Dropbox (Personal)/2022/2022-freelance/nacionalRe/20220119 VidaNr/webpack-vidaNr/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B0D0F8-3675-2C41-9040-C5AE58DCC99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336E0A24-CFE2-824C-BB57-23AB559B04BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26160" yWindow="2040" windowWidth="25860" windowHeight="17080" xr2:uid="{264BACEB-9783-544A-B5AF-004F4D7AD9C4}"/>
+    <workbookView xWindow="6920" yWindow="4620" windowWidth="25860" windowHeight="17080" xr2:uid="{264BACEB-9783-544A-B5AF-004F4D7AD9C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="338">
   <si>
     <t>key</t>
   </si>
@@ -61,15 +61,9 @@
     <t>Hombre</t>
   </si>
   <si>
-    <t>Man</t>
-  </si>
-  <si>
     <t>Mujer</t>
   </si>
   <si>
-    <t>Woman</t>
-  </si>
-  <si>
     <t>birth_date</t>
   </si>
   <si>
@@ -778,9 +772,6 @@
     <t>Insurance surcharge calculator</t>
   </si>
   <si>
-    <t>Body Mass Index </t>
-  </si>
-  <si>
     <t>h_consult_date</t>
   </si>
   <si>
@@ -880,9 +871,6 @@
     <t>índice de masa muscular</t>
   </si>
   <si>
-    <t>body mass index </t>
-  </si>
-  <si>
     <t>cerveza</t>
   </si>
   <si>
@@ -895,12 +883,6 @@
     <t>wine</t>
   </si>
   <si>
-    <t>Wine</t>
-  </si>
-  <si>
-    <t>Vino</t>
-  </si>
-  <si>
     <t>pipa</t>
   </si>
   <si>
@@ -1046,6 +1028,30 @@
   </si>
   <si>
     <t>Second blood plessure</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Mass Index</t>
+  </si>
+  <si>
+    <t>Mass Index </t>
+  </si>
+  <si>
+    <t>spirit</t>
+  </si>
+  <si>
+    <t>spirits</t>
+  </si>
+  <si>
+    <t>Vinos</t>
+  </si>
+  <si>
+    <t>Wines</t>
   </si>
 </sst>
 </file>
@@ -1408,8 +1414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6179227-BC3E-1D40-997E-5AA5DC3817CB}">
   <dimension ref="A1:C133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1433,508 +1439,508 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>9</v>
+        <v>331</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1950,937 +1956,937 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>280</v>
+        <v>332</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>294</v>
+        <v>334</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>317</v>
+        <v>335</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>7</v>
+        <v>330</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>246</v>
+        <v>333</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="C100" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="C117" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B121" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="C121" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C126" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B129" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>286</v>
+        <v>336</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>285</v>
+        <v>337</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>